<commit_message>
adjust to Isetan DMX/Ethernet Device
</commit_message>
<xml_diff>
--- a/LedAddress.xlsx
+++ b/LedAddress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1480" windowWidth="31660" windowHeight="19520"/>
+    <workbookView xWindow="2920" yWindow="1940" windowWidth="31660" windowHeight="19520"/>
   </bookViews>
   <sheets>
     <sheet name="Fill_class" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="12">
   <si>
     <t>ODE id</t>
     <phoneticPr fontId="1"/>
@@ -134,6 +134,75 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="232317"/>
+          <a:ext cx="10671098" cy="1626220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="50000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L19"/>
+  <dimension ref="A2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:L19"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -945,8 +1014,262 @@
         <v>31</v>
       </c>
     </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24">
+        <f>G24+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <f>G24+7</f>
+        <v>7</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25:L29" si="4">G25+1</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G29" si="5">G25+7</f>
+        <v>14</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27" t="s">
+        <v>8</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" t="s">
+        <v>8</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="H29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" t="s">
+        <v>8</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>